<commit_message>
Added Offset times from PremPro
</commit_message>
<xml_diff>
--- a/Study2Analysis/Study2HazardSheet.xlsx
+++ b/Study2Analysis/Study2HazardSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\OneDrive - University of Glasgow\Documents\R_Scripts\Study2Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6FAF8FD-DE37-43B6-91DE-E4EE803DDD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E329BA8-3D31-43A7-9646-91C00EC3CC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -914,7 +914,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -963,11 +963,11 @@
         <v>22.18</v>
       </c>
       <c r="E2" s="12">
-        <v>25</v>
+        <v>25.3</v>
       </c>
       <c r="F2" s="12">
         <f>E2-D2</f>
-        <v>2.8200000000000003</v>
+        <v>3.120000000000001</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>9</v>
@@ -987,11 +987,11 @@
         <v>34.43</v>
       </c>
       <c r="E3" s="12">
-        <v>40</v>
+        <v>37.616666666666667</v>
       </c>
       <c r="F3" s="12">
         <f t="shared" ref="F3:F25" si="0">E3-D3</f>
-        <v>5.57</v>
+        <v>3.1866666666666674</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>21</v>
@@ -1011,11 +1011,11 @@
         <v>22.45</v>
       </c>
       <c r="E4" s="12">
-        <v>27</v>
+        <v>32.4</v>
       </c>
       <c r="F4" s="12">
         <f t="shared" si="0"/>
-        <v>4.5500000000000007</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>21</v>
@@ -1035,11 +1035,11 @@
         <v>13.94</v>
       </c>
       <c r="E5" s="15">
-        <v>19</v>
+        <v>19.166666666666668</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="0"/>
-        <v>5.0600000000000005</v>
+        <v>5.2266666666666683</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>1</v>
@@ -1059,11 +1059,11 @@
         <v>12.42</v>
       </c>
       <c r="E6" s="15">
-        <v>16</v>
+        <v>16.283333333333335</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="0"/>
-        <v>3.58</v>
+        <v>3.8633333333333351</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>1</v>
@@ -1083,11 +1083,11 @@
         <v>29.72</v>
       </c>
       <c r="E7" s="15">
-        <v>33</v>
+        <v>33.966666666666669</v>
       </c>
       <c r="F7" s="12">
         <f t="shared" si="0"/>
-        <v>3.2800000000000011</v>
+        <v>4.2466666666666697</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>1</v>
@@ -1107,11 +1107,11 @@
         <v>34.909999999999997</v>
       </c>
       <c r="E8" s="15">
-        <v>40</v>
+        <v>40.466666666666669</v>
       </c>
       <c r="F8" s="12">
         <f t="shared" si="0"/>
-        <v>5.0900000000000034</v>
+        <v>5.556666666666672</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>21</v>
@@ -1131,11 +1131,11 @@
         <v>41.93</v>
       </c>
       <c r="E9" s="15">
-        <v>47</v>
+        <v>46.983333333333334</v>
       </c>
       <c r="F9" s="12">
         <f t="shared" si="0"/>
-        <v>5.07</v>
+        <v>5.0533333333333346</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>27</v>
@@ -1155,11 +1155,11 @@
         <v>16.82</v>
       </c>
       <c r="E10" s="15">
-        <v>20</v>
+        <v>20.133333333333333</v>
       </c>
       <c r="F10" s="12">
         <f t="shared" si="0"/>
-        <v>3.1799999999999997</v>
+        <v>3.3133333333333326</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>9</v>
@@ -1179,11 +1179,11 @@
         <v>31.75</v>
       </c>
       <c r="E11" s="15">
-        <v>36</v>
+        <v>36.06666666666667</v>
       </c>
       <c r="F11" s="12">
         <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>4.31666666666667</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>1</v>
@@ -1203,11 +1203,11 @@
         <v>22</v>
       </c>
       <c r="E12" s="12">
-        <v>26</v>
+        <v>26.383333333333333</v>
       </c>
       <c r="F12" s="12">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.3833333333333329</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>27</v>
@@ -1227,11 +1227,11 @@
         <v>26.6</v>
       </c>
       <c r="E13" s="12">
-        <v>29</v>
+        <v>29.65</v>
       </c>
       <c r="F13" s="12">
         <f t="shared" si="0"/>
-        <v>2.3999999999999986</v>
+        <v>3.0499999999999972</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>45</v>
@@ -1251,11 +1251,11 @@
         <v>20.8</v>
       </c>
       <c r="E14" s="15">
-        <v>24</v>
+        <v>25.116666666666667</v>
       </c>
       <c r="F14" s="12">
         <f t="shared" si="0"/>
-        <v>3.1999999999999993</v>
+        <v>4.3166666666666664</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>45</v>
@@ -1275,11 +1275,11 @@
         <v>9.59</v>
       </c>
       <c r="E15" s="15">
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="F15" s="12">
         <f t="shared" si="0"/>
-        <v>2.41</v>
+        <v>3.3100000000000005</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>21</v>
@@ -1299,11 +1299,11 @@
         <v>16.82</v>
       </c>
       <c r="E16" s="15">
-        <v>20</v>
+        <v>20.566666666666666</v>
       </c>
       <c r="F16" s="12">
         <f t="shared" si="0"/>
-        <v>3.1799999999999997</v>
+        <v>3.7466666666666661</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>45</v>
@@ -1323,11 +1323,11 @@
         <v>12.78</v>
       </c>
       <c r="E17" s="15">
-        <v>15</v>
+        <v>15.633333333333333</v>
       </c>
       <c r="F17" s="12">
         <f t="shared" si="0"/>
-        <v>2.2200000000000006</v>
+        <v>2.8533333333333335</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>45</v>
@@ -1347,11 +1347,11 @@
         <v>11.1</v>
       </c>
       <c r="E18" s="15">
-        <v>15</v>
+        <v>16.383333333333333</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="0"/>
-        <v>3.9000000000000004</v>
+        <v>5.2833333333333332</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>45</v>
@@ -1371,11 +1371,11 @@
         <v>27.91</v>
       </c>
       <c r="E19" s="15">
-        <v>33</v>
+        <v>33.583333333333336</v>
       </c>
       <c r="F19" s="12">
         <f t="shared" si="0"/>
-        <v>5.09</v>
+        <v>5.6733333333333356</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>1</v>
@@ -1395,11 +1395,11 @@
         <v>24.2</v>
       </c>
       <c r="E20" s="12">
-        <v>27</v>
+        <v>27.65</v>
       </c>
       <c r="F20" s="12">
         <f t="shared" si="0"/>
-        <v>2.8000000000000007</v>
+        <v>3.4499999999999993</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>9</v>
@@ -1419,11 +1419,11 @@
         <v>8</v>
       </c>
       <c r="E21" s="15">
-        <v>13</v>
+        <v>13.8</v>
       </c>
       <c r="F21" s="12">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>5.8000000000000007</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>54</v>
@@ -1443,11 +1443,11 @@
         <v>22.66</v>
       </c>
       <c r="E22" s="15">
-        <v>28</v>
+        <v>28.833333333333332</v>
       </c>
       <c r="F22" s="12">
         <f t="shared" si="0"/>
-        <v>5.34</v>
+        <v>6.173333333333332</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>1</v>
@@ -1467,11 +1467,11 @@
         <v>20.72</v>
       </c>
       <c r="E23" s="15">
-        <v>25</v>
+        <v>25.633333333333333</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" si="0"/>
-        <v>4.2800000000000011</v>
+        <v>4.913333333333334</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>9</v>
@@ -1491,11 +1491,11 @@
         <v>15.82</v>
       </c>
       <c r="E24" s="15">
-        <v>17</v>
+        <v>18.05</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="0"/>
-        <v>1.1799999999999997</v>
+        <v>2.2300000000000004</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>9</v>
@@ -1515,11 +1515,11 @@
         <v>35.479999999999997</v>
       </c>
       <c r="E25" s="15">
-        <v>39</v>
+        <v>39.583333333333336</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="0"/>
-        <v>3.5200000000000031</v>
+        <v>4.1033333333333388</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>27</v>
@@ -3272,12 +3272,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3504,15 +3501,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66466595-0D70-48C4-B5B6-0C0F2615D7E8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CCE11DE-8F59-4B9D-9CEC-424AF89C284E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="5ba15730-8bbe-4159-a04e-a72d427227a3"/>
+    <ds:schemaRef ds:uri="44914097-1524-4490-9514-e8f9bb07db88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3537,18 +3546,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CCE11DE-8F59-4B9D-9CEC-424AF89C284E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66466595-0D70-48C4-B5B6-0C0F2615D7E8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="5ba15730-8bbe-4159-a04e-a72d427227a3"/>
-    <ds:schemaRef ds:uri="44914097-1524-4490-9514-e8f9bb07db88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>